<commit_message>
modified Self Evaluation Protocol
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UKnowNothingJonSnow\Desktop\Issue-Tracking-System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UKnowNothingJonSnow\Desktop\Issue-Tracking-System\Issue-Tracking-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>16</v>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="4">
         <v>20</v>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="C32" s="10">
         <f>SUM(C6:C31)</f>
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D32" s="10">
         <v>330</v>

</xml_diff>

<commit_message>
edited self evaluation protocol
</commit_message>
<xml_diff>
--- a/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -653,7 +653,7 @@
   <dimension ref="B2:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>16</v>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="C32" s="10">
         <f>SUM(C6:C31)</f>
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D32" s="10">
         <v>330</v>

</xml_diff>